<commit_message>
All analysis page added and also download functionality of "Patient Admitted in Watchlist Hospitals"
</commit_message>
<xml_diff>
--- a/data/Suspicious_Hospital_List.xlsx
+++ b/data/Suspicious_Hospital_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ADRI\PM_JAY_Fraud_Det_Dashboard\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ADRI\Projects\pmjay_fraud_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDF6823-5C88-4CAF-9D6F-ACA28862D159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CC3BC2-AB13-48AD-9A2D-2F57E10015C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6DA63553-76CC-4127-AF95-03E79995AEE8}"/>
   </bookViews>
@@ -593,8 +593,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -650,10 +650,10 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -667,10 +667,10 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
@@ -684,10 +684,10 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -701,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
@@ -718,10 +718,10 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.3">
@@ -735,10 +735,10 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -752,10 +752,10 @@
         <v>14</v>
       </c>
       <c r="D9">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -769,10 +769,10 @@
         <v>16</v>
       </c>
       <c r="D10">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -786,10 +786,10 @@
         <v>14</v>
       </c>
       <c r="D11">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -803,10 +803,10 @@
         <v>18</v>
       </c>
       <c r="D12">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
@@ -820,10 +820,10 @@
         <v>20</v>
       </c>
       <c r="D13">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -837,10 +837,10 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
@@ -854,13 +854,13 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>28</v>
       </c>
@@ -871,13 +871,13 @@
         <v>29</v>
       </c>
       <c r="D16">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -888,10 +888,10 @@
         <v>32</v>
       </c>
       <c r="D17">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>